<commit_message>
fix: Update agenda normalization to include ENFERMERIA variations in regex patterns
</commit_message>
<xml_diff>
--- a/datos/csv_procesado/agendas_consolidadas.xlsx
+++ b/datos/csv_procesado/agendas_consolidadas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20091" uniqueCount="3188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20131" uniqueCount="3188">
   <si>
     <t>agenda_id</t>
   </si>
@@ -38831,6 +38831,9 @@
       <c r="B1007" t="s">
         <v>1836</v>
       </c>
+      <c r="D1007" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1007" t="s">
         <v>3070</v>
       </c>
@@ -38851,6 +38854,9 @@
       <c r="B1008" t="s">
         <v>1836</v>
       </c>
+      <c r="D1008" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1008" t="s">
         <v>3069</v>
       </c>
@@ -38871,6 +38877,9 @@
       <c r="B1009" t="s">
         <v>1836</v>
       </c>
+      <c r="D1009" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1009" t="s">
         <v>3067</v>
       </c>
@@ -38891,6 +38900,9 @@
       <c r="B1010" t="s">
         <v>1836</v>
       </c>
+      <c r="D1010" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1010" t="s">
         <v>3066</v>
       </c>
@@ -38911,6 +38923,9 @@
       <c r="B1011" t="s">
         <v>1836</v>
       </c>
+      <c r="D1011" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1011" t="s">
         <v>3068</v>
       </c>
@@ -38931,6 +38946,9 @@
       <c r="B1012" t="s">
         <v>1836</v>
       </c>
+      <c r="D1012" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1012" t="s">
         <v>3073</v>
       </c>
@@ -40658,6 +40676,9 @@
       <c r="B1076" t="s">
         <v>1836</v>
       </c>
+      <c r="D1076" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1076" t="s">
         <v>3070</v>
       </c>
@@ -40678,6 +40699,9 @@
       <c r="B1077" t="s">
         <v>1836</v>
       </c>
+      <c r="D1077" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1077" t="s">
         <v>3069</v>
       </c>
@@ -40698,6 +40722,9 @@
       <c r="B1078" t="s">
         <v>1836</v>
       </c>
+      <c r="D1078" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1078" t="s">
         <v>3067</v>
       </c>
@@ -40718,6 +40745,9 @@
       <c r="B1079" t="s">
         <v>1836</v>
       </c>
+      <c r="D1079" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1079" t="s">
         <v>3066</v>
       </c>
@@ -40738,6 +40768,9 @@
       <c r="B1080" t="s">
         <v>1836</v>
       </c>
+      <c r="D1080" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1080" t="s">
         <v>3068</v>
       </c>
@@ -40758,6 +40791,9 @@
       <c r="B1081" t="s">
         <v>1836</v>
       </c>
+      <c r="D1081" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1081" t="s">
         <v>3073</v>
       </c>
@@ -41964,6 +42000,9 @@
       <c r="B1126" t="s">
         <v>1836</v>
       </c>
+      <c r="D1126" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1126" t="s">
         <v>3070</v>
       </c>
@@ -41984,6 +42023,9 @@
       <c r="B1127" t="s">
         <v>1836</v>
       </c>
+      <c r="D1127" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1127" t="s">
         <v>3069</v>
       </c>
@@ -42004,6 +42046,9 @@
       <c r="B1128" t="s">
         <v>1836</v>
       </c>
+      <c r="D1128" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1128" t="s">
         <v>3067</v>
       </c>
@@ -42024,6 +42069,9 @@
       <c r="B1129" t="s">
         <v>1836</v>
       </c>
+      <c r="D1129" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1129" t="s">
         <v>3066</v>
       </c>
@@ -42044,6 +42092,9 @@
       <c r="B1130" t="s">
         <v>1836</v>
       </c>
+      <c r="D1130" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1130" t="s">
         <v>3068</v>
       </c>
@@ -42064,6 +42115,9 @@
       <c r="B1131" t="s">
         <v>1836</v>
       </c>
+      <c r="D1131" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1131" t="s">
         <v>3073</v>
       </c>
@@ -42662,6 +42716,9 @@
       <c r="B1154" t="s">
         <v>1836</v>
       </c>
+      <c r="D1154" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1154" t="s">
         <v>3070</v>
       </c>
@@ -42682,6 +42739,9 @@
       <c r="B1155" t="s">
         <v>1836</v>
       </c>
+      <c r="D1155" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1155" t="s">
         <v>3069</v>
       </c>
@@ -42702,6 +42762,9 @@
       <c r="B1156" t="s">
         <v>1836</v>
       </c>
+      <c r="D1156" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1156" t="s">
         <v>3067</v>
       </c>
@@ -42722,6 +42785,9 @@
       <c r="B1157" t="s">
         <v>1836</v>
       </c>
+      <c r="D1157" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1157" t="s">
         <v>3066</v>
       </c>
@@ -42742,6 +42808,9 @@
       <c r="B1158" t="s">
         <v>1836</v>
       </c>
+      <c r="D1158" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1158" t="s">
         <v>3068</v>
       </c>
@@ -42762,6 +42831,9 @@
       <c r="B1159" t="s">
         <v>1836</v>
       </c>
+      <c r="D1159" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1159" t="s">
         <v>3073</v>
       </c>
@@ -44752,6 +44824,9 @@
       <c r="B1236" t="s">
         <v>1930</v>
       </c>
+      <c r="D1236" t="s">
+        <v>1836</v>
+      </c>
       <c r="E1236" t="s">
         <v>3057</v>
       </c>
@@ -44775,6 +44850,9 @@
       <c r="B1237" t="s">
         <v>1930</v>
       </c>
+      <c r="D1237" t="s">
+        <v>1836</v>
+      </c>
       <c r="E1237" t="s">
         <v>3057</v>
       </c>
@@ -44798,6 +44876,9 @@
       <c r="B1238" t="s">
         <v>1930</v>
       </c>
+      <c r="D1238" t="s">
+        <v>1836</v>
+      </c>
       <c r="E1238" t="s">
         <v>3057</v>
       </c>
@@ -44821,6 +44902,9 @@
       <c r="B1239" t="s">
         <v>1930</v>
       </c>
+      <c r="D1239" t="s">
+        <v>1836</v>
+      </c>
       <c r="E1239" t="s">
         <v>3057</v>
       </c>
@@ -44844,6 +44928,9 @@
       <c r="B1240" t="s">
         <v>1930</v>
       </c>
+      <c r="D1240" t="s">
+        <v>1836</v>
+      </c>
       <c r="E1240" t="s">
         <v>3057</v>
       </c>
@@ -44867,6 +44954,9 @@
       <c r="B1241" t="s">
         <v>1930</v>
       </c>
+      <c r="D1241" t="s">
+        <v>1836</v>
+      </c>
       <c r="E1241" t="s">
         <v>3057</v>
       </c>
@@ -51125,6 +51215,9 @@
       <c r="B1484" t="s">
         <v>1836</v>
       </c>
+      <c r="D1484" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1484" t="s">
         <v>3070</v>
       </c>
@@ -51145,6 +51238,9 @@
       <c r="B1485" t="s">
         <v>1836</v>
       </c>
+      <c r="D1485" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1485" t="s">
         <v>3069</v>
       </c>
@@ -51165,6 +51261,9 @@
       <c r="B1486" t="s">
         <v>1836</v>
       </c>
+      <c r="D1486" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1486" t="s">
         <v>3067</v>
       </c>
@@ -51185,6 +51284,9 @@
       <c r="B1487" t="s">
         <v>1836</v>
       </c>
+      <c r="D1487" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1487" t="s">
         <v>3066</v>
       </c>
@@ -51205,6 +51307,9 @@
       <c r="B1488" t="s">
         <v>1836</v>
       </c>
+      <c r="D1488" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1488" t="s">
         <v>3068</v>
       </c>
@@ -52109,6 +52214,9 @@
       <c r="B1523" t="s">
         <v>2030</v>
       </c>
+      <c r="D1523" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1523" t="s">
         <v>3070</v>
       </c>
@@ -52129,6 +52237,9 @@
       <c r="B1524" t="s">
         <v>2030</v>
       </c>
+      <c r="D1524" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1524" t="s">
         <v>3069</v>
       </c>
@@ -52149,6 +52260,9 @@
       <c r="B1525" t="s">
         <v>2030</v>
       </c>
+      <c r="D1525" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1525" t="s">
         <v>3067</v>
       </c>
@@ -52169,6 +52283,9 @@
       <c r="B1526" t="s">
         <v>2030</v>
       </c>
+      <c r="D1526" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1526" t="s">
         <v>3066</v>
       </c>
@@ -52188,6 +52305,9 @@
       </c>
       <c r="B1527" t="s">
         <v>2030</v>
+      </c>
+      <c r="D1527" t="s">
+        <v>1836</v>
       </c>
       <c r="F1527" t="s">
         <v>3068</v>

</xml_diff>

<commit_message>
Update agendas_consolidadas.xlsx with new processed data
</commit_message>
<xml_diff>
--- a/datos/csv_procesado/agendas_consolidadas.xlsx
+++ b/datos/csv_procesado/agendas_consolidadas.xlsx
@@ -43,2383 +43,2383 @@
     <t>efector</t>
   </si>
   <si>
-    <t>Hospital de Clínicas San Ignacio_001_ALERGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_002_ALERGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_003_ALERGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_004_ALERGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_005_ALERGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_006_ANESTESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_007_ANESTESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_008_ANESTESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_009_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_010_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_011_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_012_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_013_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_014_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_015_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_016_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_017_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_018_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_019_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_020_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_021_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_022_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_023_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_024_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_025_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_026_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_027_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_028_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_029_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_030_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_031_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_032_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_033_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_034_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_035_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_036_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_037_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_038_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_039_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_040_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_041_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_042_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_043_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_044_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_045_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_046_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_047_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_048_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_049_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_050_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_051_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_052_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_053_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_054_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_055_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_056_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_057_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_058_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_059_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_060_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_061_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_062_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_063_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_064_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_065_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_066_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_067_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_068_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_069_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_070_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_071_CIRUGIA VASCULAR PERIFERICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_072_CIRUGIA VASCULAR PERIFERICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_073_CIRUGIA VASCULAR PERIFERICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_074_CIRUGIA VASCULAR PERIFERICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_075_CIRUGIA VASCULAR PERIFERICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_076_CIRUGIA VASCULAR PERIFERICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_077_CIRUGIA VASCULAR PERIFERICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_078_CIRUGIA VASCULAR PERIFERICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_079_CIRUGIA VASCULAR PERIFERICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_080_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_081_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_082_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_083_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_084_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_085_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_086_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_087_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_088_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_089_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_090_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_091_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_092_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_093_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_094_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_095_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_096_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_097_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_098_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_099_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_100_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_101_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_102_CUIDADOS PALIATIVOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_103_CUIDADOS PALIATIVOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_104_CUIDADOS PALIATIVOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_105_CUIDADOS PALIATIVOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_106_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_107_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_108_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_109_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_110_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_111_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_112_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_113_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_114_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_115_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_116_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_117_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_118_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_119_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_120_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_121_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_122_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_123_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_124_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_125_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_126_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_127_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_128_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_129_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_130_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_131_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_132_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_133_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_134_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_135_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_136_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_137_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_138_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_139_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_140_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_141_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_142_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_143_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_144_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_145_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_146_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_147_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_148_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_149_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_150_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_151_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_152_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_153_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_154_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_155_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_156_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_157_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_158_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_159_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_160_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_161_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_162_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_163_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_164_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_165_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_166_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_167_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_168_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_169_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_170_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_171_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_172_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_173_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_174_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_175_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_176_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_177_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_178_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_179_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_180_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_181_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_182_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_183_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_184_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_185_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_186_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_187_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_188_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_189_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_190_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_191_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_192_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_193_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_194_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_195_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_196_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_197_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_198_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_199_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_200_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_201_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_202_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_203_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_204_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_205_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_206_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_207_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_208_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_209_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_210_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_211_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_212_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_213_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_214_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_215_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_216_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_217_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_218_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_219_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_220_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_221_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_222_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_223_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_224_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_225_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_226_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_227_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_228_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_229_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_230_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_231_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_232_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_233_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_234_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_235_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_236_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_237_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_238_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_239_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_240_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_241_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_242_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_243_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_244_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_245_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_246_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_247_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_248_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_249_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_250_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_251_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_252_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_253_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_254_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_255_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_256_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_257_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_258_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_259_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_260_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_261_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_262_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_263_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_264_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_265_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_266_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_267_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_268_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_269_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_270_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_271_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_272_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_273_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_274_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_275_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_276_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_277_HEPATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_278_INFECTOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_279_INFECTOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_280_INFECTOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_281_INFECTOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_282_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_283_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_284_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_285_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_286_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_287_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_288_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_289_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_290_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_291_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_292_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_293_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_294_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_295_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_296_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_297_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_298_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_299_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_300_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_301_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_302_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_303_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_304_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_305_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_306_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_307_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_308_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_309_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_310_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_311_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_312_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_313_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_314_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_315_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_316_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_317_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_318_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_319_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_320_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_321_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_322_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_323_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_324_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_325_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_326_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_327_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_328_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_329_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_330_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_331_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_332_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_333_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_334_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_335_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_336_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_337_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_338_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_339_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_340_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_341_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_342_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_343_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_344_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_345_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_346_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_347_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_348_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_349_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_350_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_351_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_352_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_353_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_354_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_355_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_356_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_357_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_358_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_359_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_360_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_361_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_362_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_363_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_364_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_365_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_366_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_367_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_368_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_369_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_370_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_371_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_372_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_373_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_374_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_375_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_376_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_377_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_378_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_379_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_380_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_381_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_382_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_383_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_384_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_385_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_386_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_387_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_388_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_389_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_390_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_391_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_392_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_393_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_394_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_395_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_396_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_397_LABORATORIO</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_398_LABORATORIO</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_399_LABORATORIO</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_400_LABORATORIO</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_401_LABORATORIO</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_402_NEFROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_403_NEFROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_404_NEFROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_405_NEFROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_406_NEFROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_407_NEFROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_408_NEFROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_409_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_410_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_411_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_412_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_413_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_414_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_415_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_416_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_417_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_418_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_419_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_420_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_421_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_422_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_423_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_424_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_425_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_426_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_427_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_428_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_429_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_430_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_431_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_432_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_433_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_434_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_435_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_436_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_437_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_438_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_439_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_440_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_441_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_442_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_443_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_444_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_445_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_446_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_447_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_448_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_449_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_450_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_451_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_452_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_453_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_454_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_455_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_456_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_457_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_458_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_459_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_460_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_461_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_462_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_463_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_464_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_465_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_466_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_467_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_468_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_469_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_470_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_471_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_472_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_473_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_474_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_475_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_476_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_477_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_478_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_479_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_480_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_481_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_482_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_483_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_484_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_485_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_486_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_487_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_488_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_489_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_490_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_491_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_492_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_493_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_494_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_495_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_496_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_497_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_498_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_499_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_500_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_501_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_502_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_503_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_504_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_505_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_506_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_507_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_508_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_509_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_510_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_511_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_512_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_513_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_514_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_515_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_516_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_517_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_518_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_519_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_520_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_521_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_522_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_523_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_524_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_525_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_526_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_527_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_528_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_529_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_530_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_531_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_532_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_533_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_534_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_535_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_536_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_537_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_538_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_539_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_540_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_541_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_542_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_543_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_544_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_545_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_546_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_547_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_548_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_549_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_550_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_551_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_552_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_553_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_554_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_555_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_556_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_557_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_558_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_559_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_560_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_561_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_562_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_563_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_564_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_565_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_566_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_567_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_568_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_569_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_570_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_571_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_572_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_573_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_574_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_575_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_576_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_577_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_578_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_579_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_580_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_581_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_582_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_583_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_584_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_585_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_586_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_587_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_588_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_589_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_590_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_591_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_592_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_593_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_594_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_595_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_596_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_597_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_598_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_599_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_600_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_601_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_602_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_603_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_604_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_605_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_606_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_607_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_608_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_609_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_610_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_611_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_612_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_613_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_614_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_615_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_616_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_617_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_618_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_619_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_620_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_621_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_622_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_623_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_624_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_625_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_626_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_627_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_628_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_629_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_630_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_631_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_632_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_633_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_634_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_635_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_636_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_637_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_638_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_639_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_640_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_641_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_642_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_643_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_644_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_645_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_646_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_647_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_648_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_649_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_650_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_651_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_652_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_653_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_654_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_655_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_656_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_657_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_658_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_659_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_660_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_661_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_662_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_663_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_664_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_665_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_666_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_667_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_668_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_669_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_670_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_671_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_672_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_673_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_674_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_675_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_676_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_677_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_678_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_679_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_680_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_681_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_682_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_683_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_684_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_685_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_686_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_687_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_688_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_689_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_690_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_691_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_692_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_693_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_694_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_695_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_696_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_697_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_698_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_699_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_700_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_701_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_702_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_703_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_704_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_705_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_706_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_707_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_708_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_709_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_710_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_711_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_712_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_713_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_714_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_715_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_716_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_717_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_718_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_719_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_720_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_721_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_722_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_723_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_724_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_725_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_726_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_727_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_728_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_729_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_730_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_731_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_732_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_733_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_734_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_735_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_736_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_737_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_738_TBC</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_739_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_740_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_741_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_742_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_743_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_744_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_745_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_746_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_747_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_748_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_749_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_750_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_751_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_752_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_753_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_754_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_755_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_756_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_757_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_758_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_759_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_760_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_761_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_762_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_763_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_764_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_765_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_766_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_767_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_768_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_769_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_770_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_771_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_772_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_773_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_774_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_775_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_776_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_777_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_778_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_779_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_780_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_781_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_782_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_783_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_784_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_785_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_786_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_787_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_788_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_789_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_790_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_791_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_792_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_793_UROLOGÍA</t>
+    <t>HCSI_001_ALERGIA</t>
+  </si>
+  <si>
+    <t>HCSI_002_ALERGIA</t>
+  </si>
+  <si>
+    <t>HCSI_003_ALERGIA</t>
+  </si>
+  <si>
+    <t>HCSI_004_ALERGIA</t>
+  </si>
+  <si>
+    <t>HCSI_005_ALERGIA</t>
+  </si>
+  <si>
+    <t>HCSI_006_ANESTESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_007_ANESTESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_008_ANESTESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_009_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_010_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_011_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_012_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_013_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_014_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_015_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_016_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_017_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_018_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_019_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_020_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_021_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_022_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_023_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_024_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_025_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_026_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_027_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_028_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_029_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_030_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_031_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_032_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_033_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_034_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_035_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_036_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_037_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_038_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_039_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_040_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_041_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_042_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_043_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_044_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_045_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_046_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_047_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_048_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_049_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_050_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_051_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_052_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_053_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_054_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_055_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_056_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_057_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_058_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_059_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_060_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_061_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_062_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_063_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_064_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_065_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_066_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_067_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_068_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_069_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_070_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_071_CIRUGIA VASCULAR PERIFERICA</t>
+  </si>
+  <si>
+    <t>HCSI_072_CIRUGIA VASCULAR PERIFERICA</t>
+  </si>
+  <si>
+    <t>HCSI_073_CIRUGIA VASCULAR PERIFERICA</t>
+  </si>
+  <si>
+    <t>HCSI_074_CIRUGIA VASCULAR PERIFERICA</t>
+  </si>
+  <si>
+    <t>HCSI_075_CIRUGIA VASCULAR PERIFERICA</t>
+  </si>
+  <si>
+    <t>HCSI_076_CIRUGIA VASCULAR PERIFERICA</t>
+  </si>
+  <si>
+    <t>HCSI_077_CIRUGIA VASCULAR PERIFERICA</t>
+  </si>
+  <si>
+    <t>HCSI_078_CIRUGIA VASCULAR PERIFERICA</t>
+  </si>
+  <si>
+    <t>HCSI_079_CIRUGIA VASCULAR PERIFERICA</t>
+  </si>
+  <si>
+    <t>HCSI_080_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_081_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_082_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_083_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_084_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_085_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_086_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_087_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_088_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_089_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_090_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_091_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_092_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_093_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_094_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_095_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_096_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_097_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_098_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_099_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_100_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_101_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_102_CUIDADOS PALIATIVOS</t>
+  </si>
+  <si>
+    <t>HCSI_103_CUIDADOS PALIATIVOS</t>
+  </si>
+  <si>
+    <t>HCSI_104_CUIDADOS PALIATIVOS</t>
+  </si>
+  <si>
+    <t>HCSI_105_CUIDADOS PALIATIVOS</t>
+  </si>
+  <si>
+    <t>HCSI_106_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_107_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_108_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_109_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_110_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_111_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_112_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_113_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_114_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_115_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_116_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_117_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_118_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_119_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_120_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_121_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_122_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_123_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_124_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_125_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_126_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_127_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_128_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_129_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_130_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_131_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_132_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_133_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_134_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_135_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_136_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_137_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_138_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_139_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_140_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_141_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_142_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_143_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_144_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_145_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_146_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_147_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_148_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_149_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_150_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_151_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_152_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_153_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_154_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_155_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_156_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_157_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_158_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_159_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_160_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_161_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_162_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_163_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_164_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_165_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_166_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_167_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_168_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_169_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_170_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_171_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_172_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_173_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_174_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_175_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_176_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_177_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_178_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_179_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_180_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_181_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_182_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_183_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_184_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_185_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_186_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_187_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_188_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_189_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_190_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_191_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_192_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_193_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_194_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_195_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_196_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_197_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_198_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_199_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_200_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_201_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_202_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_203_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_204_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_205_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_206_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_207_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_208_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_209_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_210_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_211_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_212_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_213_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_214_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_215_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_216_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_217_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_218_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_219_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_220_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_221_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_222_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_223_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_224_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_225_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_226_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_227_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_228_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_229_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_230_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_231_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_232_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_233_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_234_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_235_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_236_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_237_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_238_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_239_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_240_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_241_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_242_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_243_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_244_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_245_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_246_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_247_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_248_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_249_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_250_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_251_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_252_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_253_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_254_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_255_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_256_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_257_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_258_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_259_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_260_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_261_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_262_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_263_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_264_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_265_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_266_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_267_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_268_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_269_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_270_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_271_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_272_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_273_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_274_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_275_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_276_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_277_HEPATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_278_INFECTOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_279_INFECTOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_280_INFECTOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_281_INFECTOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_282_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_283_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_284_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_285_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_286_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_287_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_288_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_289_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_290_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_291_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_292_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_293_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_294_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_295_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_296_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_297_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_298_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_299_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_300_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_301_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_302_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_303_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_304_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_305_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_306_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_307_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_308_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_309_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_310_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_311_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_312_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_313_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_314_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_315_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_316_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_317_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_318_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_319_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_320_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_321_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_322_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_323_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_324_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_325_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_326_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_327_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_328_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_329_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_330_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_331_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_332_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_333_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_334_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_335_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_336_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_337_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_338_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_339_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_340_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_341_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_342_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_343_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_344_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_345_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_346_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_347_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_348_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_349_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_350_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_351_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_352_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_353_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_354_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_355_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_356_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_357_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_358_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_359_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_360_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_361_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_362_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_363_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_364_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_365_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_366_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_367_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_368_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_369_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_370_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_371_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_372_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_373_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_374_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_375_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_376_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_377_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_378_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_379_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_380_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_381_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_382_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_383_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_384_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_385_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_386_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_387_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_388_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_389_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_390_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_391_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_392_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_393_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_394_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_395_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_396_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_397_LABORATORIO</t>
+  </si>
+  <si>
+    <t>HCSI_398_LABORATORIO</t>
+  </si>
+  <si>
+    <t>HCSI_399_LABORATORIO</t>
+  </si>
+  <si>
+    <t>HCSI_400_LABORATORIO</t>
+  </si>
+  <si>
+    <t>HCSI_401_LABORATORIO</t>
+  </si>
+  <si>
+    <t>HCSI_402_NEFROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_403_NEFROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_404_NEFROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_405_NEFROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_406_NEFROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_407_NEFROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_408_NEFROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_409_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_410_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_411_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_412_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_413_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_414_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_415_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_416_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_417_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_418_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_419_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_420_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_421_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_422_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_423_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_424_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_425_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_426_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_427_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_428_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_429_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_430_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_431_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_432_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_433_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_434_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_435_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_436_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_437_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_438_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_439_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_440_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_441_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_442_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_443_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_444_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_445_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_446_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_447_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_448_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_449_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_450_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_451_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_452_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_453_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_454_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_455_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_456_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_457_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_458_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_459_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_460_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_461_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_462_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_463_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_464_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_465_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_466_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_467_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_468_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_469_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_470_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_471_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_472_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_473_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_474_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_475_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_476_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_477_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_478_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_479_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_480_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_481_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_482_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_483_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_484_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_485_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_486_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_487_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_488_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_489_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_490_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_491_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_492_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_493_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_494_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_495_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_496_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_497_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_498_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_499_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_500_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_501_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_502_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_503_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_504_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_505_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_506_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_507_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_508_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_509_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_510_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_511_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_512_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_513_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_514_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_515_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_516_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_517_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_518_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_519_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_520_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_521_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_522_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_523_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_524_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_525_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_526_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_527_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_528_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_529_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_530_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_531_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_532_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_533_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_534_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_535_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_536_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_537_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_538_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_539_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_540_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_541_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_542_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_543_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_544_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_545_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_546_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_547_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_548_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_549_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_550_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_551_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_552_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_553_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_554_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_555_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_556_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_557_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_558_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_559_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_560_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_561_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_562_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_563_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_564_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_565_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_566_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_567_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_568_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_569_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_570_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_571_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_572_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_573_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_574_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_575_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_576_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_577_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_578_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_579_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_580_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_581_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_582_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_583_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_584_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_585_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_586_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_587_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_588_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_589_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_590_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_591_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_592_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_593_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_594_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_595_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_596_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_597_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_598_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_599_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_600_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_601_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_602_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_603_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_604_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_605_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_606_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_607_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_608_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_609_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_610_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_611_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_612_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_613_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_614_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_615_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_616_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_617_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_618_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_619_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_620_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_621_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_622_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_623_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_624_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_625_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_626_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_627_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_628_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_629_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_630_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_631_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_632_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_633_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_634_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_635_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_636_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_637_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_638_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_639_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_640_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_641_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_642_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_643_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_644_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_645_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_646_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_647_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_648_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_649_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_650_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_651_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_652_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_653_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_654_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_655_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_656_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_657_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_658_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_659_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_660_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_661_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_662_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_663_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_664_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_665_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_666_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_667_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_668_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_669_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_670_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_671_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_672_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_673_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_674_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_675_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_676_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_677_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_678_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_679_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_680_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_681_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_682_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_683_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_684_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_685_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_686_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_687_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_688_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_689_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_690_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_691_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_692_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_693_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_694_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_695_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_696_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_697_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_698_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_699_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_700_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_701_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_702_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_703_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_704_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_705_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_706_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_707_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_708_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_709_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_710_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_711_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_712_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_713_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_714_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_715_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_716_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_717_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_718_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_719_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_720_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_721_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_722_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_723_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_724_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_725_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_726_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_727_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_728_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_729_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_730_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_731_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_732_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_733_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_734_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_735_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_736_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_737_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_738_TBC</t>
+  </si>
+  <si>
+    <t>HCSI_739_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_740_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_741_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_742_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_743_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_744_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_745_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_746_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_747_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_748_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_749_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_750_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_751_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_752_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_753_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_754_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_755_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_756_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_757_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_758_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_759_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_760_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_761_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_762_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_763_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_764_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_765_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_766_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_767_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_768_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_769_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_770_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_771_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_772_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_773_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_774_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_775_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_776_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_777_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_778_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_779_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_780_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_781_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_782_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_783_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_784_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_785_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_786_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_787_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_788_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_789_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_790_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_791_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_792_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_793_UROLOGÍA</t>
   </si>
   <si>
     <t>CAPS Bajo Boulogne_002_PEDIATRIA - DRA. CHIFFLET MARIA - PROGRAMADA</t>
@@ -9538,7 +9538,7 @@
     <t>10:10</t>
   </si>
   <si>
-    <t>Hospital de Clínicas San Ignacio</t>
+    <t>HCSI</t>
   </si>
   <si>
     <t>CAPS Bajo Boulogne</t>

</xml_diff>

<commit_message>
Restauración. Eliminé los filtros múltiples
</commit_message>
<xml_diff>
--- a/datos/csv_procesado/agendas_consolidadas.xlsx
+++ b/datos/csv_procesado/agendas_consolidadas.xlsx
@@ -43,2383 +43,2383 @@
     <t>efector</t>
   </si>
   <si>
-    <t>Hospital de Clínicas San Ignacio_001_ALERGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_002_ALERGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_003_ALERGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_004_ALERGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_005_ALERGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_006_ANESTESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_007_ANESTESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_008_ANESTESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_009_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_010_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_011_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_012_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_013_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_014_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_015_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_016_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_017_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_018_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_019_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_020_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_021_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_022_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_023_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_024_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_025_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_026_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_027_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_028_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_029_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_030_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_031_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_032_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_033_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_034_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_035_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_036_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_037_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_038_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_039_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_040_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_041_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_042_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_043_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_044_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_045_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_046_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_047_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_048_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_049_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_050_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_051_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_052_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_053_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_054_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_055_CARDIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_056_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_057_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_058_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_059_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_060_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_061_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_062_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_063_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_064_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_065_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_066_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_067_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_068_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_069_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_070_CIRUGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_071_CIRUGIA VASCULAR PERIFERICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_072_CIRUGIA VASCULAR PERIFERICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_073_CIRUGIA VASCULAR PERIFERICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_074_CIRUGIA VASCULAR PERIFERICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_075_CIRUGIA VASCULAR PERIFERICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_076_CIRUGIA VASCULAR PERIFERICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_077_CIRUGIA VASCULAR PERIFERICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_078_CIRUGIA VASCULAR PERIFERICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_079_CIRUGIA VASCULAR PERIFERICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_080_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_081_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_082_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_083_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_084_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_085_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_086_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_087_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_088_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_089_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_090_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_091_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_092_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_093_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_094_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_095_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_096_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_097_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_098_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_099_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_100_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_101_CLINICA MEDICA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_102_CUIDADOS PALIATIVOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_103_CUIDADOS PALIATIVOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_104_CUIDADOS PALIATIVOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_105_CUIDADOS PALIATIVOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_106_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_107_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_108_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_109_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_110_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_111_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_112_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_113_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_114_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_115_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_116_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_117_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_118_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_119_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_120_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_121_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_122_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_123_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_124_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_125_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_126_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_127_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_128_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_129_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_130_DERMATOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_131_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_132_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_133_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_134_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_135_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_136_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_137_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_138_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_139_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_140_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_141_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_142_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_143_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_144_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_145_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_146_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_147_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_148_DIABETOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_149_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_150_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_151_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_152_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_153_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_154_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_155_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_156_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_157_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_158_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_159_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_160_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_161_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_162_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_163_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_164_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_165_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_166_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_167_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_168_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_169_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_170_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_171_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_172_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_173_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_174_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_175_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_176_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_177_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_178_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_179_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_180_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_181_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_182_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_183_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_184_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_185_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_186_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_187_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_188_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_189_DIAGNOSTICO POR IMAGENES</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_190_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_191_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_192_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_193_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_194_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_195_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_196_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_197_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_198_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_199_DISCAPACIDAD</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_200_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_201_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_202_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_203_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_204_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_205_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_206_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_207_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_208_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_209_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_210_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_211_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_212_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_213_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_214_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_215_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_216_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_217_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_218_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_219_ENDOCRINOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_220_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_221_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_222_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_223_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_224_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_225_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_226_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_227_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_228_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_229_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_230_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_231_GASTROENTEROLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_232_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_233_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_234_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_235_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_236_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_237_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_238_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_239_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_240_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_241_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_242_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_243_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_244_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_245_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_246_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_247_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_248_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_249_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_250_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_251_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_252_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_253_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_254_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_255_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_256_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_257_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_258_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_259_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_260_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_261_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_262_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_263_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_264_GINECOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_265_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_266_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_267_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_268_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_269_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_270_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_271_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_272_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_273_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_274_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_275_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_276_HEMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_277_HEPATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_278_INFECTOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_279_INFECTOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_280_INFECTOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_281_INFECTOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_282_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_283_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_284_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_285_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_286_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_287_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_288_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_289_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_290_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_291_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_292_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_293_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_294_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_295_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_296_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_297_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_298_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_299_INTERNADOS</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_300_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_301_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_302_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_303_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_304_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_305_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_306_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_307_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_308_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_309_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_310_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_311_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_312_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_313_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_314_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_315_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_316_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_317_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_318_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_319_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_320_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_321_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_322_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_323_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_324_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_325_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_326_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_327_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_328_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_329_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_330_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_331_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_332_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_333_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_334_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_335_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_336_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_337_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_338_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_339_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_340_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_341_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_342_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_343_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_344_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_345_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_346_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_347_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_348_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_349_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_350_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_351_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_352_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_353_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_354_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_355_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_356_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_357_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_358_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_359_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_360_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_361_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_362_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_363_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_364_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_365_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_366_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_367_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_368_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_369_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_370_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_371_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_372_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_373_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_374_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_375_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_376_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_377_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_378_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_379_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_380_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_381_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_382_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_383_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_384_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_385_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_386_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_387_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_388_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_389_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_390_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_391_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_392_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_393_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_394_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_395_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_396_KINESIOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_397_LABORATORIO</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_398_LABORATORIO</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_399_LABORATORIO</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_400_LABORATORIO</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_401_LABORATORIO</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_402_NEFROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_403_NEFROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_404_NEFROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_405_NEFROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_406_NEFROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_407_NEFROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_408_NEFROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_409_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_410_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_411_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_412_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_413_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_414_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_415_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_416_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_417_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_418_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_419_NEUMONOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_420_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_421_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_422_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_423_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_424_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_425_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_426_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_427_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_428_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_429_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_430_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_431_NEUROCIRUGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_432_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_433_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_434_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_435_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_436_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_437_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_438_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_439_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_440_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_441_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_442_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_443_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_444_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_445_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_446_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_447_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_448_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_449_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_450_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_451_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_452_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_453_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_454_NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_455_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_456_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_457_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_458_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_459_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_460_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_461_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_462_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_463_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_464_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_465_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_466_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_467_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_468_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_469_NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_470_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_471_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_472_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_473_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_474_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_475_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_476_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_477_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_478_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_479_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_480_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_481_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_482_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_483_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_484_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_485_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_486_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_487_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_488_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_489_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_490_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_491_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_492_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_493_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_494_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_495_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_496_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_497_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_498_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_499_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_500_OFTALMOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_501_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_502_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_503_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_504_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_505_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_506_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_507_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_508_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_509_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_510_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_511_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_512_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_513_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_514_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_515_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_516_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_517_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_518_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_519_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_520_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_521_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_522_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_523_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_524_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_525_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_526_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_527_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_528_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_529_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_530_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_531_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_532_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_533_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_534_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_535_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_536_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_537_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_538_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_539_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_540_ONCOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_541_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_542_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_543_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_544_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_545_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_546_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_547_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_548_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_549_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_550_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_551_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_552_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_553_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_554_OTORRINOLARINGOLOGIA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_555_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_556_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_557_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_558_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_559_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_560_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_561_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_562_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_563_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_564_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_565_REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_566_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_567_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_568_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_569_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_570_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_571_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_572_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_573_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_574_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_575_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_576_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_577_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_578_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_579_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_580_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_581_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_582_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_583_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_584_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_585_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_586_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_587_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_588_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_589_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_590_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_591_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_592_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_593_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_594_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_595_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_596_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_597_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_598_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_599_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_600_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_601_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_602_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_603_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_604_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_605_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_606_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_607_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_608_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_609_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_610_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_611_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_612_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_613_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_614_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_615_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_616_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_617_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_618_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_619_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_620_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_621_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_622_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_623_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_624_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_625_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_626_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_627_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_628_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_629_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_630_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_631_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_632_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_633_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_634_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_635_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_636_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_637_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_638_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_639_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_640_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_641_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_642_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_643_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_644_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_645_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_646_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_647_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_648_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_649_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_650_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_651_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_652_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_653_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_654_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_655_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_656_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_657_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_658_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_659_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_660_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_661_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_662_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_663_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_664_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_665_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_666_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_667_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_668_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_669_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_670_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_671_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_672_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_673_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_674_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_675_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_676_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_677_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_678_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_679_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_680_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_681_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_682_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_683_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_684_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_685_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_686_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_687_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_688_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_689_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_690_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_691_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_692_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_693_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_694_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_695_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_696_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_697_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_698_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_699_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_700_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_701_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_702_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_703_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_704_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_705_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_706_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_707_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_708_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_709_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_710_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_711_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_712_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_713_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_714_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_715_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_716_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_717_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_718_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_719_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_720_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_721_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_722_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_723_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_724_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_725_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_726_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_727_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_728_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_729_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_730_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_731_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_732_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_733_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_734_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_735_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_736_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_737_SALUD MENTAL</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_738_TBC</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_739_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_740_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_741_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_742_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_743_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_744_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_745_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_746_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_747_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_748_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_749_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_750_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_751_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_752_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_753_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_754_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_755_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_756_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_757_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_758_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_759_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_760_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_761_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_762_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_763_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_764_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_765_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_766_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_767_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_768_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_769_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_770_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_771_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_772_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_773_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_774_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_775_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_776_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_777_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_778_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_779_TRAUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_780_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_781_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_782_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_783_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_784_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_785_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_786_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_787_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_788_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_789_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_790_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_791_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_792_UROLOGÍA</t>
-  </si>
-  <si>
-    <t>Hospital de Clínicas San Ignacio_793_UROLOGÍA</t>
+    <t>HCSI_001_ALERGIA</t>
+  </si>
+  <si>
+    <t>HCSI_002_ALERGIA</t>
+  </si>
+  <si>
+    <t>HCSI_003_ALERGIA</t>
+  </si>
+  <si>
+    <t>HCSI_004_ALERGIA</t>
+  </si>
+  <si>
+    <t>HCSI_005_ALERGIA</t>
+  </si>
+  <si>
+    <t>HCSI_006_ANESTESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_007_ANESTESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_008_ANESTESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_009_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_010_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_011_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_012_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_013_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_014_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_015_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_016_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_017_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_018_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_019_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_020_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_021_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_022_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_023_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_024_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_025_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_026_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_027_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_028_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_029_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_030_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_031_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_032_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_033_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_034_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_035_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_036_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_037_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_038_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_039_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_040_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_041_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_042_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_043_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_044_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_045_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_046_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_047_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_048_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_049_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_050_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_051_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_052_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_053_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_054_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_055_CARDIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_056_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_057_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_058_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_059_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_060_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_061_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_062_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_063_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_064_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_065_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_066_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_067_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_068_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_069_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_070_CIRUGIA</t>
+  </si>
+  <si>
+    <t>HCSI_071_CIRUGIA VASCULAR PERIFERICA</t>
+  </si>
+  <si>
+    <t>HCSI_072_CIRUGIA VASCULAR PERIFERICA</t>
+  </si>
+  <si>
+    <t>HCSI_073_CIRUGIA VASCULAR PERIFERICA</t>
+  </si>
+  <si>
+    <t>HCSI_074_CIRUGIA VASCULAR PERIFERICA</t>
+  </si>
+  <si>
+    <t>HCSI_075_CIRUGIA VASCULAR PERIFERICA</t>
+  </si>
+  <si>
+    <t>HCSI_076_CIRUGIA VASCULAR PERIFERICA</t>
+  </si>
+  <si>
+    <t>HCSI_077_CIRUGIA VASCULAR PERIFERICA</t>
+  </si>
+  <si>
+    <t>HCSI_078_CIRUGIA VASCULAR PERIFERICA</t>
+  </si>
+  <si>
+    <t>HCSI_079_CIRUGIA VASCULAR PERIFERICA</t>
+  </si>
+  <si>
+    <t>HCSI_080_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_081_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_082_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_083_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_084_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_085_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_086_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_087_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_088_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_089_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_090_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_091_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_092_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_093_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_094_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_095_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_096_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_097_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_098_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_099_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_100_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_101_CLINICA MEDICA</t>
+  </si>
+  <si>
+    <t>HCSI_102_CUIDADOS PALIATIVOS</t>
+  </si>
+  <si>
+    <t>HCSI_103_CUIDADOS PALIATIVOS</t>
+  </si>
+  <si>
+    <t>HCSI_104_CUIDADOS PALIATIVOS</t>
+  </si>
+  <si>
+    <t>HCSI_105_CUIDADOS PALIATIVOS</t>
+  </si>
+  <si>
+    <t>HCSI_106_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_107_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_108_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_109_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_110_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_111_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_112_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_113_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_114_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_115_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_116_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_117_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_118_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_119_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_120_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_121_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_122_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_123_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_124_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_125_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_126_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_127_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_128_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_129_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_130_DERMATOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_131_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_132_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_133_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_134_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_135_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_136_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_137_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_138_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_139_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_140_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_141_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_142_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_143_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_144_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_145_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_146_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_147_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_148_DIABETOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_149_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_150_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_151_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_152_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_153_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_154_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_155_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_156_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_157_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_158_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_159_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_160_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_161_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_162_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_163_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_164_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_165_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_166_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_167_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_168_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_169_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_170_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_171_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_172_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_173_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_174_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_175_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_176_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_177_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_178_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_179_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_180_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_181_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_182_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_183_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_184_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_185_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_186_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_187_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_188_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_189_DIAGNOSTICO POR IMAGENES</t>
+  </si>
+  <si>
+    <t>HCSI_190_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_191_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_192_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_193_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_194_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_195_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_196_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_197_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_198_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_199_DISCAPACIDAD</t>
+  </si>
+  <si>
+    <t>HCSI_200_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_201_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_202_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_203_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_204_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_205_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_206_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_207_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_208_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_209_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_210_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_211_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_212_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_213_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_214_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_215_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_216_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_217_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_218_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_219_ENDOCRINOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_220_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_221_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_222_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_223_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_224_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_225_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_226_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_227_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_228_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_229_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_230_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_231_GASTROENTEROLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_232_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_233_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_234_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_235_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_236_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_237_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_238_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_239_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_240_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_241_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_242_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_243_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_244_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_245_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_246_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_247_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_248_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_249_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_250_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_251_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_252_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_253_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_254_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_255_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_256_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_257_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_258_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_259_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_260_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_261_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_262_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_263_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_264_GINECOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_265_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_266_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_267_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_268_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_269_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_270_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_271_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_272_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_273_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_274_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_275_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_276_HEMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_277_HEPATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_278_INFECTOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_279_INFECTOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_280_INFECTOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_281_INFECTOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_282_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_283_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_284_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_285_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_286_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_287_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_288_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_289_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_290_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_291_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_292_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_293_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_294_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_295_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_296_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_297_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_298_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_299_INTERNADOS</t>
+  </si>
+  <si>
+    <t>HCSI_300_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_301_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_302_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_303_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_304_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_305_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_306_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_307_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_308_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_309_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_310_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_311_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_312_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_313_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_314_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_315_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_316_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_317_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_318_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_319_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_320_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_321_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_322_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_323_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_324_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_325_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_326_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_327_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_328_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_329_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_330_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_331_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_332_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_333_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_334_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_335_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_336_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_337_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_338_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_339_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_340_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_341_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_342_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_343_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_344_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_345_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_346_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_347_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_348_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_349_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_350_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_351_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_352_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_353_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_354_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_355_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_356_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_357_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_358_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_359_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_360_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_361_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_362_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_363_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_364_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_365_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_366_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_367_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_368_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_369_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_370_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_371_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_372_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_373_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_374_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_375_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_376_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_377_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_378_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_379_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_380_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_381_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_382_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_383_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_384_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_385_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_386_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_387_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_388_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_389_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_390_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_391_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_392_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_393_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_394_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_395_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_396_KINESIOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_397_LABORATORIO</t>
+  </si>
+  <si>
+    <t>HCSI_398_LABORATORIO</t>
+  </si>
+  <si>
+    <t>HCSI_399_LABORATORIO</t>
+  </si>
+  <si>
+    <t>HCSI_400_LABORATORIO</t>
+  </si>
+  <si>
+    <t>HCSI_401_LABORATORIO</t>
+  </si>
+  <si>
+    <t>HCSI_402_NEFROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_403_NEFROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_404_NEFROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_405_NEFROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_406_NEFROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_407_NEFROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_408_NEFROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_409_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_410_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_411_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_412_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_413_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_414_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_415_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_416_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_417_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_418_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_419_NEUMONOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_420_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_421_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_422_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_423_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_424_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_425_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_426_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_427_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_428_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_429_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_430_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_431_NEUROCIRUGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_432_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_433_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_434_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_435_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_436_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_437_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_438_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_439_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_440_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_441_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_442_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_443_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_444_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_445_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_446_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_447_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_448_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_449_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_450_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_451_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_452_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_453_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_454_NEUROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_455_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_456_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_457_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_458_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_459_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_460_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_461_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_462_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_463_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_464_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_465_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_466_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_467_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_468_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_469_NUTRICIÓN</t>
+  </si>
+  <si>
+    <t>HCSI_470_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_471_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_472_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_473_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_474_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_475_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_476_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_477_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_478_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_479_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_480_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_481_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_482_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_483_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_484_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_485_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_486_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_487_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_488_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_489_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_490_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_491_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_492_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_493_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_494_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_495_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_496_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_497_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_498_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_499_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_500_OFTALMOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_501_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_502_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_503_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_504_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_505_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_506_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_507_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_508_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_509_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_510_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_511_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_512_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_513_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_514_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_515_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_516_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_517_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_518_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_519_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_520_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_521_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_522_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_523_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_524_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_525_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_526_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_527_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_528_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_529_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_530_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_531_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_532_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_533_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_534_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_535_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_536_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_537_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_538_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_539_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_540_ONCOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_541_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_542_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_543_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_544_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_545_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_546_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_547_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_548_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_549_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_550_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_551_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_552_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_553_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_554_OTORRINOLARINGOLOGIA</t>
+  </si>
+  <si>
+    <t>HCSI_555_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_556_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_557_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_558_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_559_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_560_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_561_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_562_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_563_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_564_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_565_REUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_566_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_567_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_568_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_569_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_570_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_571_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_572_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_573_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_574_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_575_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_576_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_577_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_578_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_579_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_580_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_581_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_582_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_583_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_584_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_585_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_586_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_587_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_588_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_589_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_590_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_591_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_592_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_593_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_594_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_595_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_596_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_597_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_598_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_599_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_600_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_601_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_602_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_603_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_604_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_605_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_606_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_607_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_608_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_609_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_610_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_611_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_612_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_613_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_614_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_615_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_616_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_617_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_618_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_619_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_620_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_621_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_622_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_623_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_624_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_625_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_626_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_627_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_628_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_629_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_630_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_631_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_632_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_633_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_634_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_635_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_636_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_637_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_638_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_639_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_640_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_641_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_642_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_643_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_644_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_645_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_646_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_647_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_648_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_649_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_650_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_651_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_652_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_653_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_654_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_655_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_656_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_657_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_658_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_659_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_660_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_661_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_662_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_663_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_664_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_665_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_666_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_667_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_668_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_669_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_670_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_671_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_672_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_673_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_674_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_675_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_676_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_677_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_678_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_679_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_680_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_681_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_682_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_683_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_684_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_685_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_686_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_687_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_688_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_689_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_690_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_691_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_692_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_693_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_694_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_695_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_696_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_697_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_698_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_699_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_700_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_701_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_702_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_703_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_704_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_705_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_706_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_707_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_708_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_709_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_710_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_711_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_712_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_713_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_714_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_715_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_716_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_717_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_718_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_719_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_720_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_721_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_722_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_723_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_724_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_725_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_726_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_727_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_728_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_729_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_730_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_731_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_732_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_733_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_734_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_735_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_736_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_737_SALUD MENTAL</t>
+  </si>
+  <si>
+    <t>HCSI_738_TBC</t>
+  </si>
+  <si>
+    <t>HCSI_739_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_740_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_741_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_742_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_743_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_744_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_745_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_746_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_747_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_748_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_749_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_750_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_751_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_752_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_753_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_754_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_755_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_756_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_757_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_758_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_759_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_760_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_761_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_762_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_763_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_764_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_765_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_766_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_767_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_768_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_769_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_770_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_771_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_772_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_773_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_774_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_775_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_776_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_777_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_778_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_779_TRAUMATOLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_780_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_781_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_782_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_783_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_784_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_785_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_786_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_787_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_788_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_789_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_790_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_791_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_792_UROLOGÍA</t>
+  </si>
+  <si>
+    <t>HCSI_793_UROLOGÍA</t>
   </si>
   <si>
     <t>CAPS Bajo Boulogne_002_PEDIATRIA - DRA. CHIFFLET MARIA - PROGRAMADA</t>
@@ -9538,7 +9538,7 @@
     <t>10:10</t>
   </si>
   <si>
-    <t>Hospital de Clínicas San Ignacio</t>
+    <t>HCSI</t>
   </si>
   <si>
     <t>CAPS Bajo Boulogne</t>

</xml_diff>

<commit_message>
feat: Add SIGLAS_REFERENCIA.md for acronym documentation and refactor agenda filters for improved usability
</commit_message>
<xml_diff>
--- a/datos/csv_procesado/agendas_consolidadas.xlsx
+++ b/datos/csv_procesado/agendas_consolidadas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20091" uniqueCount="3188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20131" uniqueCount="3188">
   <si>
     <t>agenda_id</t>
   </si>
@@ -38831,6 +38831,9 @@
       <c r="B1007" t="s">
         <v>1836</v>
       </c>
+      <c r="D1007" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1007" t="s">
         <v>3070</v>
       </c>
@@ -38851,6 +38854,9 @@
       <c r="B1008" t="s">
         <v>1836</v>
       </c>
+      <c r="D1008" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1008" t="s">
         <v>3069</v>
       </c>
@@ -38871,6 +38877,9 @@
       <c r="B1009" t="s">
         <v>1836</v>
       </c>
+      <c r="D1009" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1009" t="s">
         <v>3067</v>
       </c>
@@ -38891,6 +38900,9 @@
       <c r="B1010" t="s">
         <v>1836</v>
       </c>
+      <c r="D1010" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1010" t="s">
         <v>3066</v>
       </c>
@@ -38911,6 +38923,9 @@
       <c r="B1011" t="s">
         <v>1836</v>
       </c>
+      <c r="D1011" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1011" t="s">
         <v>3068</v>
       </c>
@@ -38931,6 +38946,9 @@
       <c r="B1012" t="s">
         <v>1836</v>
       </c>
+      <c r="D1012" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1012" t="s">
         <v>3073</v>
       </c>
@@ -40658,6 +40676,9 @@
       <c r="B1076" t="s">
         <v>1836</v>
       </c>
+      <c r="D1076" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1076" t="s">
         <v>3070</v>
       </c>
@@ -40678,6 +40699,9 @@
       <c r="B1077" t="s">
         <v>1836</v>
       </c>
+      <c r="D1077" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1077" t="s">
         <v>3069</v>
       </c>
@@ -40698,6 +40722,9 @@
       <c r="B1078" t="s">
         <v>1836</v>
       </c>
+      <c r="D1078" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1078" t="s">
         <v>3067</v>
       </c>
@@ -40718,6 +40745,9 @@
       <c r="B1079" t="s">
         <v>1836</v>
       </c>
+      <c r="D1079" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1079" t="s">
         <v>3066</v>
       </c>
@@ -40738,6 +40768,9 @@
       <c r="B1080" t="s">
         <v>1836</v>
       </c>
+      <c r="D1080" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1080" t="s">
         <v>3068</v>
       </c>
@@ -40758,6 +40791,9 @@
       <c r="B1081" t="s">
         <v>1836</v>
       </c>
+      <c r="D1081" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1081" t="s">
         <v>3073</v>
       </c>
@@ -41964,6 +42000,9 @@
       <c r="B1126" t="s">
         <v>1836</v>
       </c>
+      <c r="D1126" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1126" t="s">
         <v>3070</v>
       </c>
@@ -41984,6 +42023,9 @@
       <c r="B1127" t="s">
         <v>1836</v>
       </c>
+      <c r="D1127" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1127" t="s">
         <v>3069</v>
       </c>
@@ -42004,6 +42046,9 @@
       <c r="B1128" t="s">
         <v>1836</v>
       </c>
+      <c r="D1128" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1128" t="s">
         <v>3067</v>
       </c>
@@ -42024,6 +42069,9 @@
       <c r="B1129" t="s">
         <v>1836</v>
       </c>
+      <c r="D1129" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1129" t="s">
         <v>3066</v>
       </c>
@@ -42044,6 +42092,9 @@
       <c r="B1130" t="s">
         <v>1836</v>
       </c>
+      <c r="D1130" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1130" t="s">
         <v>3068</v>
       </c>
@@ -42064,6 +42115,9 @@
       <c r="B1131" t="s">
         <v>1836</v>
       </c>
+      <c r="D1131" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1131" t="s">
         <v>3073</v>
       </c>
@@ -42662,6 +42716,9 @@
       <c r="B1154" t="s">
         <v>1836</v>
       </c>
+      <c r="D1154" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1154" t="s">
         <v>3070</v>
       </c>
@@ -42682,6 +42739,9 @@
       <c r="B1155" t="s">
         <v>1836</v>
       </c>
+      <c r="D1155" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1155" t="s">
         <v>3069</v>
       </c>
@@ -42702,6 +42762,9 @@
       <c r="B1156" t="s">
         <v>1836</v>
       </c>
+      <c r="D1156" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1156" t="s">
         <v>3067</v>
       </c>
@@ -42722,6 +42785,9 @@
       <c r="B1157" t="s">
         <v>1836</v>
       </c>
+      <c r="D1157" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1157" t="s">
         <v>3066</v>
       </c>
@@ -42742,6 +42808,9 @@
       <c r="B1158" t="s">
         <v>1836</v>
       </c>
+      <c r="D1158" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1158" t="s">
         <v>3068</v>
       </c>
@@ -42762,6 +42831,9 @@
       <c r="B1159" t="s">
         <v>1836</v>
       </c>
+      <c r="D1159" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1159" t="s">
         <v>3073</v>
       </c>
@@ -44752,6 +44824,9 @@
       <c r="B1236" t="s">
         <v>1930</v>
       </c>
+      <c r="D1236" t="s">
+        <v>1836</v>
+      </c>
       <c r="E1236" t="s">
         <v>3057</v>
       </c>
@@ -44775,6 +44850,9 @@
       <c r="B1237" t="s">
         <v>1930</v>
       </c>
+      <c r="D1237" t="s">
+        <v>1836</v>
+      </c>
       <c r="E1237" t="s">
         <v>3057</v>
       </c>
@@ -44798,6 +44876,9 @@
       <c r="B1238" t="s">
         <v>1930</v>
       </c>
+      <c r="D1238" t="s">
+        <v>1836</v>
+      </c>
       <c r="E1238" t="s">
         <v>3057</v>
       </c>
@@ -44821,6 +44902,9 @@
       <c r="B1239" t="s">
         <v>1930</v>
       </c>
+      <c r="D1239" t="s">
+        <v>1836</v>
+      </c>
       <c r="E1239" t="s">
         <v>3057</v>
       </c>
@@ -44844,6 +44928,9 @@
       <c r="B1240" t="s">
         <v>1930</v>
       </c>
+      <c r="D1240" t="s">
+        <v>1836</v>
+      </c>
       <c r="E1240" t="s">
         <v>3057</v>
       </c>
@@ -44867,6 +44954,9 @@
       <c r="B1241" t="s">
         <v>1930</v>
       </c>
+      <c r="D1241" t="s">
+        <v>1836</v>
+      </c>
       <c r="E1241" t="s">
         <v>3057</v>
       </c>
@@ -51125,6 +51215,9 @@
       <c r="B1484" t="s">
         <v>1836</v>
       </c>
+      <c r="D1484" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1484" t="s">
         <v>3070</v>
       </c>
@@ -51145,6 +51238,9 @@
       <c r="B1485" t="s">
         <v>1836</v>
       </c>
+      <c r="D1485" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1485" t="s">
         <v>3069</v>
       </c>
@@ -51165,6 +51261,9 @@
       <c r="B1486" t="s">
         <v>1836</v>
       </c>
+      <c r="D1486" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1486" t="s">
         <v>3067</v>
       </c>
@@ -51185,6 +51284,9 @@
       <c r="B1487" t="s">
         <v>1836</v>
       </c>
+      <c r="D1487" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1487" t="s">
         <v>3066</v>
       </c>
@@ -51205,6 +51307,9 @@
       <c r="B1488" t="s">
         <v>1836</v>
       </c>
+      <c r="D1488" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1488" t="s">
         <v>3068</v>
       </c>
@@ -52109,6 +52214,9 @@
       <c r="B1523" t="s">
         <v>2030</v>
       </c>
+      <c r="D1523" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1523" t="s">
         <v>3070</v>
       </c>
@@ -52129,6 +52237,9 @@
       <c r="B1524" t="s">
         <v>2030</v>
       </c>
+      <c r="D1524" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1524" t="s">
         <v>3069</v>
       </c>
@@ -52149,6 +52260,9 @@
       <c r="B1525" t="s">
         <v>2030</v>
       </c>
+      <c r="D1525" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1525" t="s">
         <v>3067</v>
       </c>
@@ -52169,6 +52283,9 @@
       <c r="B1526" t="s">
         <v>2030</v>
       </c>
+      <c r="D1526" t="s">
+        <v>1836</v>
+      </c>
       <c r="F1526" t="s">
         <v>3066</v>
       </c>
@@ -52188,6 +52305,9 @@
       </c>
       <c r="B1527" t="s">
         <v>2030</v>
+      </c>
+      <c r="D1527" t="s">
+        <v>1836</v>
       </c>
       <c r="F1527" t="s">
         <v>3068</v>

</xml_diff>